<commit_message>
Added a couple of comments.
</commit_message>
<xml_diff>
--- a/Documentation/MoPlusIdeasToTasks.xlsx
+++ b/Documentation/MoPlusIdeasToTasks.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenSource\MoPlus\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -321,6 +316,47 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Need clarification and example, is this at a project level? Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.  </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Can move source code (and Mo+ specific templates) into a SourceCode folder, is there an easy way to perform a move in tfs?</t>
+    </r>
+  </si>
+  <si>
+    <t>Needed to set projects to x86 for VSPackage installation, can revisit if there is another way to be able to install VSPackage. Will verify in Cosmos. IIRC we only set entrypoint assemblies (the ones registered to VS) to x86.</t>
+  </si>
+  <si>
+    <t>Intent is for template libraries to be shared across projects, not sure of additional overall benefits of relative path to templates.  Should be revisited when overall template management workflow is overhauled. Of course templates should be shared. But think of Nuget: "relative" paths, but locally contained shared stuff. that way the projects' dependencies are locally managed.</t>
+  </si>
+  <si>
+    <t>This is due to large forward engineering model.  Serialization based loader doesn’t report progress, whereas spec templates do report progress.  Probably wait for other overall workflow changes which may change the loading process altogether. M: at some point I'd personally go for handwritten serialization (or self-generated based on reflection information)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Address error messaging, unique based on name/node needs to remain until future workflow/language changes. M: I understand the reasoning why they need to be unique, but it should prevent me from adding a second one with a duplicate name then </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D: agree that tool should prevent template collisions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>I made some validation changes for database names, verify if any additional changes are required.</t>
     </r>
     <r>
@@ -332,104 +368,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> M: I wouldn't do any functional validation (besides possible storage limitations like max length). If users mistype, they get a provider error DB NOT FOUND. ie, dont invest in redundant checks</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Address error messaging, unique based on name/node needs to remain until future workflow/language changes. </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <u/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>M: I understand the reasoning why they need to be unique, but it should prevent me from adding a second one with a duplicate name then</t>
+      <t>M: I wouldn't do any functional validation (besides possible storage limitations like max length). If users mistype, they get a provider error DB NOT FOUND. ie, dont invest in redundant checks</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This is due to large forward engineering model.  Serialization based loader doesn’t report progress, whereas spec templates do report progress.  Probably wait for other overall workflow changes which may change the loading process altogether. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M: at some point I'd personally go for handwritten serialization (or self-generated based on reflection information)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Intent is for template libraries to be shared across projects, not sure of additional overall benefits of relative path to templates.  Should be revisited when overall template management workflow is overhauled. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Of course templates should be shared. But think of Nuget: "relative" paths, but locally contained shared stuff. that way the projects' dependencies are locally managed.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Needed to set projects to x86 for VSPackage installation, can revisit if there is another way to be able to install VSPackage. </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Will verify in Cosmos. IIRC we only set entrypoint assemblies (the ones registered to VS) to x86.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Propose scheme.</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Once we have a "bulk-insert" thing, we can do "move-up" "move-down" buttons thingy (See #7)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Need clarification and example, is this at a project level? </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.</t>
-    </r>
+    <t>Propose scheme. Once we have a "bulk-insert" thing, we can do "move-up" "move-down" buttons thingy (See #7)</t>
   </si>
 </sst>
 </file>
@@ -506,30 +459,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -552,6 +484,27 @@
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -566,25 +519,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:G42" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:G42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G42"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Idea" dataDxfId="7"/>
-    <tableColumn id="3" name="Type" dataDxfId="6"/>
-    <tableColumn id="4" name="Component" dataDxfId="5"/>
-    <tableColumn id="5" name="Projected Release" dataDxfId="4"/>
-    <tableColumn id="6" name="Who will lead next steps" dataDxfId="3"/>
-    <tableColumn id="7" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" name="ID" dataDxfId="6"/>
+    <tableColumn id="2" name="Idea" dataDxfId="5"/>
+    <tableColumn id="3" name="Type" dataDxfId="4"/>
+    <tableColumn id="4" name="Component" dataDxfId="3"/>
+    <tableColumn id="5" name="Projected Release" dataDxfId="2"/>
+    <tableColumn id="6" name="Who will lead next steps" dataDxfId="1"/>
+    <tableColumn id="7" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -622,9 +575,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,7 +612,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +647,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -871,7 +824,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1127,7 +1080,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1150,7 +1103,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1196,7 +1149,7 @@
         <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1242,7 +1195,7 @@
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1288,7 +1241,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1446,7 +1399,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added additional notes to the excel sheet
</commit_message>
<xml_diff>
--- a/Documentation/MoPlusIdeasToTasks.xlsx
+++ b/Documentation/MoPlusIdeasToTasks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenSource\MoPlus\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -312,25 +317,6 @@
     <t>Dynamic methods for performance improvement.</t>
   </si>
   <si>
-    <t>http://msdn.microsoft.com/en-us/library/exczf7b9.aspx</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Need clarification and example, is this at a project level? Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.  </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Can move source code (and Mo+ specific templates) into a SourceCode folder, is there an easy way to perform a move in tfs?</t>
-    </r>
-  </si>
-  <si>
     <t>Needed to set projects to x86 for VSPackage installation, can revisit if there is another way to be able to install VSPackage. Will verify in Cosmos. IIRC we only set entrypoint assemblies (the ones registered to VS) to x86.</t>
   </si>
   <si>
@@ -338,22 +324,6 @@
   </si>
   <si>
     <t>This is due to large forward engineering model.  Serialization based loader doesn’t report progress, whereas spec templates do report progress.  Probably wait for other overall workflow changes which may change the loading process altogether. M: at some point I'd personally go for handwritten serialization (or self-generated based on reflection information)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Address error messaging, unique based on name/node needs to remain until future workflow/language changes. M: I understand the reasoning why they need to be unique, but it should prevent me from adding a second one with a duplicate name then </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D: agree that tool should prevent template collisions.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -383,6 +353,41 @@
   </si>
   <si>
     <t>Propose scheme. Once we have a "bulk-insert" thing, we can do "move-up" "move-down" buttons thingy (See #7)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Need clarification and example, is this at a project level? Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.  Can move source code (and Mo+ specific templates) into a SourceCode folder, is there an easy way to perform a move in tfs? </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It's git specific now. best way to go is unbind the solution and projects from within vs. then do a git file move (not exactly sure how), and bind the projects again</t>
+    </r>
+  </si>
+  <si>
+    <t>Address error messaging, unique based on name/node needs to remain until future workflow/language changes. M: I understand the reasoning why they need to be unique, but it should prevent me from adding a second one with a duplicate name then. Agree that tool should prevent template collisions.</t>
+  </si>
+  <si>
+    <r>
+      <t>See http://msdn.microsoft.com/en-us/library/exczf7b9.aspx.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I'd seriously wait till we get a 60-80% test coverage, because making simple dynamic methods is doable, but the mo+ language is quite complex, so emitting dynamic methods for them is even more complex. Maybe we should use the command line solutionbuilder thing to do the template work? (update solution, update specification, etc) That way, we could just emit c# code and compile it at runtime. That would be much easier.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -459,7 +464,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -535,9 +540,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -575,9 +580,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,7 +617,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -647,7 +652,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -823,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +887,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1080,7 +1085,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1103,7 +1108,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1149,7 +1154,7 @@
         <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1195,7 +1200,7 @@
         <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1241,7 +1246,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1399,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1764,7 +1769,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>17</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved tests a bit.
</commit_message>
<xml_diff>
--- a/Documentation/MoPlusIdeasToTasks.xlsx
+++ b/Documentation/MoPlusIdeasToTasks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="100">
   <si>
     <t>Idea</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Put all sources (current files) in a top-level folder named Code or Sources, all dependencies in a top-level Dependencies or Resources. This gives you room to make more logical division of fil</t>
   </si>
   <si>
     <t>Technical</t>
@@ -388,6 +385,12 @@
       </rPr>
       <t xml:space="preserve"> I'd seriously wait till we get a 60-80% test coverage, because making simple dynamic methods is doable, but the mo+ language is quite complex, so emitting dynamic methods for them is even more complex. Maybe we should use the command line solutionbuilder thing to do the template work? (update solution, update specification, etc) That way, we could just emit c# code and compile it at runtime. That would be much easier.</t>
     </r>
+  </si>
+  <si>
+    <t>Put all sources (current files) in a top-level folder named Code or Sources, all dependencies in a top-level Dependencies or Resources. This gives you room to make more logical division of files</t>
+  </si>
+  <si>
+    <t>Mostly done already. Did a find and replace.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -460,6 +463,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -828,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +852,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -872,22 +878,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" s="4">
         <v>1.1000000000000001</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -895,22 +901,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -918,19 +924,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
+      <c r="G4" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -938,19 +947,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -958,19 +967,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -978,22 +987,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1001,22 +1010,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1024,22 +1033,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1047,22 +1056,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1070,22 +1079,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1093,22 +1102,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1116,22 +1125,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1139,22 +1148,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1162,22 +1171,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1185,22 +1194,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1208,22 +1217,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1231,22 +1240,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1254,22 +1263,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1277,19 +1286,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1297,22 +1306,22 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1320,22 +1329,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1343,22 +1352,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1366,22 +1375,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1389,22 +1398,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,22 +1421,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1435,22 +1444,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1458,22 +1467,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1481,22 +1490,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1504,22 +1513,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1527,22 +1536,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1550,22 +1559,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1573,22 +1582,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1596,22 +1605,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1619,22 +1628,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1642,22 +1651,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,22 +1674,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="G37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,19 +1697,19 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E38" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1708,19 +1717,19 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1728,22 +1737,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1751,22 +1760,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1774,22 +1783,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated version of excel sheet
</commit_message>
<xml_diff>
--- a/Documentation/MoPlusIdeasToTasks.xlsx
+++ b/Documentation/MoPlusIdeasToTasks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenSource\MoPlus\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="100">
   <si>
     <t>Idea</t>
   </si>
@@ -318,32 +323,6 @@
     <t>This is due to large forward engineering model.  Serialization based loader doesn’t report progress, whereas spec templates do report progress.  Probably wait for other overall workflow changes which may change the loading process altogether. M: at some point I'd personally go for handwritten serialization (or self-generated based on reflection information)</t>
   </si>
   <si>
-    <r>
-      <t>I made some validation changes for database names, verify if any additional changes are required.</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M: I wouldn't do any functional validation (besides possible storage limitations like max length). If users mistype, they get a provider error DB NOT FOUND. ie, dont invest in redundant checks</t>
-    </r>
-  </si>
-  <si>
     <t>Propose scheme. Once we have a "bulk-insert" thing, we can do "move-up" "move-down" buttons thingy (See #7)</t>
   </si>
   <si>
@@ -357,6 +336,12 @@
   </si>
   <si>
     <t>Need clarification and example, is this at a project level? Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.  Can move source code (and Mo+ specific templates) into a SourceCode folder, is there an easy way to perform a move in tfs? It's git specific now. best way to go is unbind the solution and projects from within vs. then do a git file move (not exactly sure how), and bind the projects again</t>
+  </si>
+  <si>
+    <t>Mostly done already. Did a find and replace.</t>
+  </si>
+  <si>
+    <t>I made some validation changes for database names, verify if any additional changes are required. M: I wouldn't do any functional validation (besides possible storage limitations like max length). If users mistype, they get a provider error DB NOT FOUND. ie, dont invest in redundant checks</t>
   </si>
 </sst>
 </file>
@@ -414,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,9 +416,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -509,9 +497,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -549,9 +537,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -586,7 +574,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,7 +609,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -797,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +844,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -901,6 +889,9 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="G4" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1054,7 +1045,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1215,7 +1206,7 @@
         <v>17</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1373,7 +1364,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1712,7 +1703,7 @@
         <v>17</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1758,7 +1749,7 @@
         <v>17</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Status update in template.
</commit_message>
<xml_diff>
--- a/Documentation/MoPlusIdeasToTasks.xlsx
+++ b/Documentation/MoPlusIdeasToTasks.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenSource\MoPlus\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
@@ -338,10 +333,30 @@
     <t>Need clarification and example, is this at a project level? Perfect sample is this excel sheet. It's mixed in with the source folders. I always have a Sources folder in the root, Dependencies, Resources, Documentation (all optional). I'd then put this spreadheet in documentation, as well as any articles, user guides, etc.  Can move source code (and Mo+ specific templates) into a SourceCode folder, is there an easy way to perform a move in tfs? It's git specific now. best way to go is unbind the solution and projects from within vs. then do a git file move (not exactly sure how), and bind the projects again</t>
   </si>
   <si>
-    <t>Mostly done already. Did a find and replace.</t>
-  </si>
-  <si>
     <t>I made some validation changes for database names, verify if any additional changes are required. M: I wouldn't do any functional validation (besides possible storage limitations like max length). If users mistype, they get a provider error DB NOT FOUND. ie, dont invest in redundant checks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mostly done already. Did a find and replace. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Updated some templates accordingly.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -421,7 +436,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -497,9 +512,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -537,9 +552,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,7 +589,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,7 +624,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -785,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1364,7 +1379,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>